<commit_message>
PROS-6581 - CCRU - new KPI tables and POS 2019 - SD-65494 SD-65488
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/KPIs for DB - PoS 2019.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/KPIs for DB - PoS 2019.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -884,10 +885,10 @@
     <t xml:space="preserve">Швеппс Шпритц - 0.25л стекло</t>
   </si>
   <si>
-    <t xml:space="preserve">New SKU 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Новый вкус 1</t>
+    <t xml:space="preserve">Schweppes Ginger Spritz - 0.25L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Имбирь - 0.25л стекло</t>
   </si>
   <si>
     <t xml:space="preserve">Sprite - 0.25L Glass/Fanta Orange - 0.25L Glass</t>
@@ -1037,97 +1038,97 @@
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - REG</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.25л стекло/Фанта Апельсин - 0.25л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 0.75L Glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 0.75л стекло</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy any</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Энергетик любой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Импульсной зоны Дисплей NRGB (бар)/Доп. выкладка от 3-х фейсингов (бар)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Активация Импульсной зоны Дисплей NRGB (бар)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Petroleum - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Pomegranate - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Гранат - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero Cherry - 0.9L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро Вишня- 0.9л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Tonic - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Тоник - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SmartWater Still - 0.6L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Смарт вода - 0.6л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Passion Punch - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Берн Тропический микс - 0.5л</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEW SKU 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 0.25л стекло/Фанта Апельсин - 0.25л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Still - 0.75L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Негаз - 0.75л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy any</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Энергетик любой</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активация Импульсной зоны Дисплей NRGB (бар)/Доп. выкладка от 3-х фейсингов (бар)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - REG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активация Импульсной зоны Дисплей NRGB (бар)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoS 2019 - IC Petroleum - CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola - 0.9L/1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Pomegranate - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Гранат - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Апельсин - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange - 0.9L/1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite - 0.9L/1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero - 0.9L/1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero Cherry - 0.9L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро Вишня- 0.9л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Tonic - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Тоник - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SmartWater Still - 0.6L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Смарт вода - 0.6л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn Passion Punch - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Берн Тропический микс - 0.5л</t>
   </si>
   <si>
     <t xml:space="preserve">Новое SKU 1</t>
@@ -2886,18 +2887,18 @@
   </sheetPr>
   <dimension ref="A1:F2008"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A310" activeCellId="0" sqref="A310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="84.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="108.397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="48.4897959183674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="23.4795918367347"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9691,7 +9692,7 @@
         <v>0.27</v>
       </c>
       <c r="D340" s="0" t="s">
-        <v>337</v>
+        <v>286</v>
       </c>
       <c r="E340" s="0" t="s">
         <v>287</v>
@@ -10142,7 +10143,7 @@
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B363" s="0" t="s">
         <v>7</v>
@@ -10162,7 +10163,7 @@
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B364" s="0" t="s">
         <v>7</v>
@@ -10182,7 +10183,7 @@
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B365" s="0" t="s">
         <v>7</v>
@@ -10202,7 +10203,7 @@
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B366" s="0" t="s">
         <v>7</v>
@@ -10222,7 +10223,7 @@
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B367" s="0" t="s">
         <v>7</v>
@@ -10242,7 +10243,7 @@
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B368" s="0" t="s">
         <v>7</v>
@@ -10251,7 +10252,7 @@
         <v>0.27</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>337</v>
+        <v>286</v>
       </c>
       <c r="E368" s="0" t="s">
         <v>287</v>
@@ -10262,7 +10263,7 @@
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B369" s="0" t="s">
         <v>7</v>
@@ -10274,7 +10275,7 @@
         <v>288</v>
       </c>
       <c r="E369" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F369" s="0" t="n">
         <v>0.02</v>
@@ -10282,7 +10283,7 @@
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B370" s="0" t="s">
         <v>54</v>
@@ -10302,7 +10303,7 @@
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B371" s="0" t="s">
         <v>54</v>
@@ -10311,10 +10312,10 @@
         <v>0.06</v>
       </c>
       <c r="D371" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="E371" s="0" t="s">
         <v>340</v>
-      </c>
-      <c r="E371" s="0" t="s">
-        <v>341</v>
       </c>
       <c r="F371" s="0" t="n">
         <v>0.01</v>
@@ -10322,7 +10323,7 @@
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B372" s="0" t="s">
         <v>219</v>
@@ -10342,7 +10343,7 @@
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B373" s="0" t="s">
         <v>219</v>
@@ -10362,7 +10363,7 @@
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B374" s="0" t="s">
         <v>219</v>
@@ -10382,7 +10383,7 @@
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B375" s="0" t="s">
         <v>219</v>
@@ -10402,7 +10403,7 @@
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B376" s="0" t="s">
         <v>219</v>
@@ -10422,7 +10423,7 @@
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B377" s="0" t="s">
         <v>219</v>
@@ -10442,7 +10443,7 @@
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B378" s="0" t="s">
         <v>219</v>
@@ -10462,7 +10463,7 @@
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B379" s="0" t="s">
         <v>219</v>
@@ -10482,7 +10483,7 @@
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B380" s="0" t="s">
         <v>67</v>
@@ -10491,10 +10492,10 @@
         <v>0.01</v>
       </c>
       <c r="D380" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="E380" s="0" t="s">
         <v>342</v>
-      </c>
-      <c r="E380" s="0" t="s">
-        <v>343</v>
       </c>
       <c r="F380" s="0" t="n">
         <v>0.01</v>
@@ -10502,7 +10503,7 @@
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B381" s="0" t="s">
         <v>310</v>
@@ -10522,7 +10523,7 @@
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B382" s="0" t="s">
         <v>312</v>
@@ -10534,7 +10535,7 @@
         <v>313</v>
       </c>
       <c r="E382" s="0" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F382" s="0" t="n">
         <v>0</v>
@@ -10542,7 +10543,7 @@
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B383" s="0" t="s">
         <v>315</v>
@@ -10562,7 +10563,7 @@
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B384" s="0" t="s">
         <v>315</v>
@@ -10582,7 +10583,7 @@
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B385" s="0" t="s">
         <v>320</v>
@@ -10602,7 +10603,7 @@
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B386" s="0" t="s">
         <v>320</v>
@@ -10622,7 +10623,7 @@
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B387" s="0" t="s">
         <v>320</v>
@@ -10642,7 +10643,7 @@
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B388" s="0" t="s">
         <v>320</v>
@@ -10662,7 +10663,7 @@
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B389" s="0" t="s">
         <v>329</v>
@@ -10682,7 +10683,7 @@
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B390" s="0" t="s">
         <v>329</v>
@@ -10702,7 +10703,7 @@
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B391" s="0" t="s">
         <v>329</v>
@@ -10722,7 +10723,7 @@
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B392" s="0" t="s">
         <v>7</v>
@@ -10742,7 +10743,7 @@
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B393" s="0" t="s">
         <v>7</v>
@@ -10762,7 +10763,7 @@
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B394" s="0" t="s">
         <v>7</v>
@@ -10782,7 +10783,7 @@
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B395" s="0" t="s">
         <v>7</v>
@@ -10802,7 +10803,7 @@
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B396" s="0" t="s">
         <v>7</v>
@@ -10822,7 +10823,7 @@
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B397" s="0" t="s">
         <v>7</v>
@@ -10834,7 +10835,7 @@
         <v>288</v>
       </c>
       <c r="E397" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F397" s="0" t="n">
         <v>0.03</v>
@@ -10842,7 +10843,7 @@
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B398" s="0" t="s">
         <v>54</v>
@@ -10862,7 +10863,7 @@
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B399" s="0" t="s">
         <v>54</v>
@@ -10871,10 +10872,10 @@
         <v>0.06</v>
       </c>
       <c r="D399" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="E399" s="0" t="s">
         <v>340</v>
-      </c>
-      <c r="E399" s="0" t="s">
-        <v>341</v>
       </c>
       <c r="F399" s="0" t="n">
         <v>0.01</v>
@@ -10882,7 +10883,7 @@
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B400" s="0" t="s">
         <v>219</v>
@@ -10902,7 +10903,7 @@
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B401" s="0" t="s">
         <v>219</v>
@@ -10922,7 +10923,7 @@
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B402" s="0" t="s">
         <v>219</v>
@@ -10942,7 +10943,7 @@
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B403" s="0" t="s">
         <v>219</v>
@@ -10962,7 +10963,7 @@
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B404" s="0" t="s">
         <v>219</v>
@@ -10982,7 +10983,7 @@
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B405" s="0" t="s">
         <v>219</v>
@@ -11002,7 +11003,7 @@
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B406" s="0" t="s">
         <v>219</v>
@@ -11022,7 +11023,7 @@
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B407" s="0" t="s">
         <v>219</v>
@@ -11042,7 +11043,7 @@
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B408" s="0" t="s">
         <v>67</v>
@@ -11051,10 +11052,10 @@
         <v>0.01</v>
       </c>
       <c r="D408" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="E408" s="0" t="s">
         <v>342</v>
-      </c>
-      <c r="E408" s="0" t="s">
-        <v>343</v>
       </c>
       <c r="F408" s="0" t="n">
         <v>0.01</v>
@@ -11062,7 +11063,7 @@
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B409" s="0" t="s">
         <v>310</v>
@@ -11082,7 +11083,7 @@
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B410" s="0" t="s">
         <v>312</v>
@@ -11094,7 +11095,7 @@
         <v>313</v>
       </c>
       <c r="E410" s="0" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F410" s="0" t="n">
         <v>0</v>
@@ -11102,7 +11103,7 @@
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B411" s="0" t="s">
         <v>315</v>
@@ -11122,7 +11123,7 @@
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B412" s="0" t="s">
         <v>315</v>
@@ -11142,7 +11143,7 @@
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B413" s="0" t="s">
         <v>320</v>
@@ -11162,7 +11163,7 @@
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B414" s="0" t="s">
         <v>320</v>
@@ -11182,7 +11183,7 @@
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B415" s="0" t="s">
         <v>320</v>
@@ -11202,7 +11203,7 @@
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B416" s="0" t="s">
         <v>320</v>
@@ -11222,7 +11223,7 @@
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B417" s="0" t="s">
         <v>329</v>
@@ -11242,7 +11243,7 @@
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B418" s="0" t="s">
         <v>329</v>
@@ -11262,7 +11263,7 @@
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B419" s="0" t="s">
         <v>329</v>
@@ -11282,7 +11283,7 @@
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B420" s="0" t="s">
         <v>7</v>
@@ -11302,7 +11303,7 @@
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B421" s="0" t="s">
         <v>7</v>
@@ -11311,7 +11312,7 @@
         <v>0.168845</v>
       </c>
       <c r="D421" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E421" s="0" t="s">
         <v>9</v>
@@ -11322,7 +11323,7 @@
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B422" s="0" t="s">
         <v>7</v>
@@ -11342,7 +11343,7 @@
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B423" s="0" t="s">
         <v>7</v>
@@ -11362,7 +11363,7 @@
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B424" s="0" t="s">
         <v>7</v>
@@ -11382,7 +11383,7 @@
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B425" s="0" t="s">
         <v>7</v>
@@ -11402,7 +11403,7 @@
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B426" s="0" t="s">
         <v>7</v>
@@ -11422,7 +11423,7 @@
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B427" s="0" t="s">
         <v>7</v>
@@ -11442,7 +11443,7 @@
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B428" s="0" t="s">
         <v>7</v>
@@ -11462,7 +11463,7 @@
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B429" s="0" t="s">
         <v>7</v>
@@ -11471,10 +11472,10 @@
         <v>0.168845</v>
       </c>
       <c r="D429" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E429" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E429" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F429" s="0" t="n">
         <v>0.007</v>
@@ -11482,7 +11483,7 @@
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B430" s="0" t="s">
         <v>7</v>
@@ -11491,10 +11492,10 @@
         <v>0.168845</v>
       </c>
       <c r="D430" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E430" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="E430" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="F430" s="0" t="n">
         <v>0.007</v>
@@ -11502,7 +11503,7 @@
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B431" s="0" t="s">
         <v>7</v>
@@ -11511,10 +11512,10 @@
         <v>0.168845</v>
       </c>
       <c r="D431" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E431" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E431" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F431" s="0" t="n">
         <v>0.005597</v>
@@ -11522,7 +11523,7 @@
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B432" s="0" t="s">
         <v>7</v>
@@ -11531,7 +11532,7 @@
         <v>0.168845</v>
       </c>
       <c r="D432" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E432" s="0" t="s">
         <v>15</v>
@@ -11542,7 +11543,7 @@
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B433" s="0" t="s">
         <v>7</v>
@@ -11551,10 +11552,10 @@
         <v>0.168845</v>
       </c>
       <c r="D433" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E433" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E433" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F433" s="0" t="n">
         <v>0.005597</v>
@@ -11562,7 +11563,7 @@
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B434" s="0" t="s">
         <v>7</v>
@@ -11582,7 +11583,7 @@
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B435" s="0" t="s">
         <v>7</v>
@@ -11591,7 +11592,7 @@
         <v>0.168845</v>
       </c>
       <c r="D435" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E435" s="0" t="s">
         <v>17</v>
@@ -11602,7 +11603,7 @@
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B436" s="0" t="s">
         <v>7</v>
@@ -11622,7 +11623,7 @@
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B437" s="0" t="s">
         <v>7</v>
@@ -11631,7 +11632,7 @@
         <v>0.168845</v>
       </c>
       <c r="D437" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E437" s="0" t="s">
         <v>35</v>
@@ -11642,7 +11643,7 @@
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B438" s="0" t="s">
         <v>7</v>
@@ -11651,10 +11652,10 @@
         <v>0.168845</v>
       </c>
       <c r="D438" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E438" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E438" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F438" s="0" t="n">
         <v>0.005597</v>
@@ -11662,7 +11663,7 @@
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B439" s="0" t="s">
         <v>7</v>
@@ -11671,10 +11672,10 @@
         <v>0.168845</v>
       </c>
       <c r="D439" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E439" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E439" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F439" s="0" t="n">
         <v>0.005597</v>
@@ -11682,7 +11683,7 @@
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B440" s="0" t="s">
         <v>7</v>
@@ -11702,7 +11703,7 @@
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B441" s="0" t="s">
         <v>54</v>
@@ -11722,7 +11723,7 @@
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B442" s="0" t="s">
         <v>54</v>
@@ -11742,7 +11743,7 @@
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B443" s="0" t="s">
         <v>54</v>
@@ -11762,7 +11763,7 @@
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B444" s="0" t="s">
         <v>54</v>
@@ -11771,10 +11772,10 @@
         <v>0.040776</v>
       </c>
       <c r="D444" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="E444" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="E444" s="0" t="s">
-        <v>365</v>
       </c>
       <c r="F444" s="0" t="n">
         <v>0.007</v>
@@ -11782,7 +11783,7 @@
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B445" s="0" t="s">
         <v>54</v>
@@ -11802,7 +11803,7 @@
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B446" s="0" t="s">
         <v>67</v>
@@ -11822,7 +11823,7 @@
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B447" s="0" t="s">
         <v>67</v>
@@ -11842,7 +11843,7 @@
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B448" s="0" t="s">
         <v>67</v>
@@ -11862,7 +11863,7 @@
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B449" s="0" t="s">
         <v>67</v>
@@ -11882,7 +11883,7 @@
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B450" s="0" t="s">
         <v>67</v>
@@ -11891,10 +11892,10 @@
         <v>0.062122</v>
       </c>
       <c r="D450" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E450" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="E450" s="0" t="s">
-        <v>367</v>
       </c>
       <c r="F450" s="0" t="n">
         <v>0.007</v>
@@ -11902,7 +11903,7 @@
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B451" s="0" t="s">
         <v>67</v>
@@ -11911,7 +11912,7 @@
         <v>0.062122</v>
       </c>
       <c r="D451" s="0" t="s">
-        <v>337</v>
+        <v>367</v>
       </c>
       <c r="E451" s="0" t="s">
         <v>368</v>
@@ -11922,7 +11923,7 @@
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B452" s="0" t="s">
         <v>78</v>
@@ -11942,7 +11943,7 @@
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B453" s="0" t="s">
         <v>78</v>
@@ -11962,7 +11963,7 @@
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B454" s="0" t="s">
         <v>78</v>
@@ -11982,7 +11983,7 @@
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B455" s="0" t="s">
         <v>78</v>
@@ -12002,7 +12003,7 @@
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B456" s="0" t="s">
         <v>78</v>
@@ -12022,7 +12023,7 @@
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B457" s="0" t="s">
         <v>78</v>
@@ -12042,7 +12043,7 @@
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B458" s="0" t="s">
         <v>219</v>
@@ -12062,7 +12063,7 @@
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B459" s="0" t="s">
         <v>219</v>
@@ -12082,7 +12083,7 @@
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B460" s="0" t="s">
         <v>219</v>
@@ -12102,7 +12103,7 @@
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B461" s="0" t="s">
         <v>219</v>
@@ -12122,7 +12123,7 @@
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B462" s="0" t="s">
         <v>219</v>
@@ -12142,7 +12143,7 @@
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B463" s="0" t="s">
         <v>219</v>
@@ -12162,7 +12163,7 @@
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B464" s="0" t="s">
         <v>219</v>
@@ -12182,7 +12183,7 @@
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B465" s="0" t="s">
         <v>219</v>
@@ -12202,7 +12203,7 @@
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B466" s="0" t="s">
         <v>219</v>
@@ -12222,7 +12223,7 @@
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B467" s="0" t="s">
         <v>219</v>
@@ -12242,7 +12243,7 @@
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B468" s="0" t="s">
         <v>384</v>
@@ -12262,7 +12263,7 @@
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B469" s="0" t="s">
         <v>386</v>
@@ -12282,7 +12283,7 @@
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B470" s="0" t="s">
         <v>388</v>
@@ -12302,7 +12303,7 @@
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B471" s="0" t="s">
         <v>390</v>
@@ -12322,7 +12323,7 @@
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B472" s="0" t="s">
         <v>390</v>
@@ -12342,7 +12343,7 @@
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B473" s="0" t="s">
         <v>390</v>
@@ -12362,7 +12363,7 @@
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B474" s="0" t="s">
         <v>390</v>
@@ -12382,7 +12383,7 @@
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B475" s="0" t="s">
         <v>151</v>
@@ -12402,7 +12403,7 @@
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B476" s="0" t="s">
         <v>151</v>
@@ -12422,7 +12423,7 @@
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B477" s="0" t="s">
         <v>158</v>
@@ -12442,7 +12443,7 @@
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B478" s="0" t="s">
         <v>175</v>
@@ -12462,7 +12463,7 @@
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B479" s="0" t="s">
         <v>160</v>
@@ -12482,7 +12483,7 @@
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B480" s="0" t="s">
         <v>396</v>
@@ -12502,7 +12503,7 @@
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B481" s="0" t="s">
         <v>396</v>
@@ -12522,7 +12523,7 @@
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B482" s="0" t="s">
         <v>396</v>
@@ -12542,7 +12543,7 @@
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B483" s="0" t="s">
         <v>396</v>
@@ -12562,7 +12563,7 @@
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B484" s="0" t="s">
         <v>396</v>
@@ -12582,7 +12583,7 @@
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B485" s="0" t="s">
         <v>396</v>
@@ -12602,7 +12603,7 @@
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B486" s="0" t="s">
         <v>409</v>
@@ -12622,7 +12623,7 @@
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B487" s="0" t="s">
         <v>411</v>
@@ -12642,7 +12643,7 @@
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B488" s="0" t="s">
         <v>413</v>
@@ -12691,7 +12692,7 @@
         <v>0.168904</v>
       </c>
       <c r="D490" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E490" s="0" t="s">
         <v>9</v>
@@ -12791,10 +12792,10 @@
         <v>0.168904</v>
       </c>
       <c r="D495" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E495" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E495" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F495" s="0" t="n">
         <v>0.007009</v>
@@ -12871,10 +12872,10 @@
         <v>0.168904</v>
       </c>
       <c r="D499" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E499" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="E499" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="F499" s="0" t="n">
         <v>0.007009</v>
@@ -12891,10 +12892,10 @@
         <v>0.168904</v>
       </c>
       <c r="D500" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E500" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E500" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F500" s="0" t="n">
         <v>0.005591</v>
@@ -12911,10 +12912,10 @@
         <v>0.168904</v>
       </c>
       <c r="D501" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E501" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E501" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F501" s="0" t="n">
         <v>0.005591</v>
@@ -12931,7 +12932,7 @@
         <v>0.168904</v>
       </c>
       <c r="D502" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E502" s="0" t="s">
         <v>35</v>
@@ -12951,7 +12952,7 @@
         <v>0.168904</v>
       </c>
       <c r="D503" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E503" s="0" t="s">
         <v>17</v>
@@ -12991,7 +12992,7 @@
         <v>0.168904</v>
       </c>
       <c r="D505" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E505" s="0" t="s">
         <v>15</v>
@@ -13051,10 +13052,10 @@
         <v>0.168904</v>
       </c>
       <c r="D508" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E508" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E508" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F508" s="0" t="n">
         <v>0.005591</v>
@@ -13251,10 +13252,10 @@
         <v>0.067668</v>
       </c>
       <c r="D518" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E518" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="E518" s="0" t="s">
-        <v>367</v>
       </c>
       <c r="F518" s="0" t="n">
         <v>0.007006</v>
@@ -13271,7 +13272,7 @@
         <v>0.067668</v>
       </c>
       <c r="D519" s="0" t="s">
-        <v>337</v>
+        <v>367</v>
       </c>
       <c r="E519" s="0" t="s">
         <v>368</v>
@@ -14631,7 +14632,7 @@
         <v>0.14901</v>
       </c>
       <c r="D587" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E587" s="0" t="s">
         <v>456</v>
@@ -14731,7 +14732,7 @@
         <v>0.14901</v>
       </c>
       <c r="D592" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E592" s="0" t="s">
         <v>457</v>
@@ -14751,7 +14752,7 @@
         <v>0.14901</v>
       </c>
       <c r="D593" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E593" s="0" t="s">
         <v>458</v>
@@ -14771,7 +14772,7 @@
         <v>0.14901</v>
       </c>
       <c r="D594" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E594" s="0" t="s">
         <v>459</v>
@@ -14871,10 +14872,10 @@
         <v>0.14901</v>
       </c>
       <c r="D599" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E599" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E599" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F599" s="0" t="n">
         <v>0.003994</v>
@@ -14931,10 +14932,10 @@
         <v>0.14901</v>
       </c>
       <c r="D602" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E602" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E602" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F602" s="0" t="n">
         <v>0.003993</v>
@@ -14971,10 +14972,10 @@
         <v>0.14901</v>
       </c>
       <c r="D604" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E604" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="E604" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="F604" s="0" t="n">
         <v>0.003993</v>
@@ -15011,10 +15012,10 @@
         <v>0.14901</v>
       </c>
       <c r="D606" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E606" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E606" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F606" s="0" t="n">
         <v>0.002995</v>
@@ -15031,10 +15032,10 @@
         <v>0.14901</v>
       </c>
       <c r="D607" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E607" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E607" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F607" s="0" t="n">
         <v>0.002995</v>
@@ -15091,10 +15092,10 @@
         <v>0.14901</v>
       </c>
       <c r="D610" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E610" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E610" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F610" s="0" t="n">
         <v>0.002995</v>
@@ -15431,10 +15432,10 @@
         <v>0.019195</v>
       </c>
       <c r="D627" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E627" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="E627" s="0" t="s">
-        <v>367</v>
       </c>
       <c r="F627" s="0" t="n">
         <v>0.001222</v>
@@ -17511,7 +17512,7 @@
         <v>0.148995</v>
       </c>
       <c r="D731" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E731" s="0" t="s">
         <v>456</v>
@@ -17611,7 +17612,7 @@
         <v>0.148995</v>
       </c>
       <c r="D736" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E736" s="0" t="s">
         <v>457</v>
@@ -17631,7 +17632,7 @@
         <v>0.148995</v>
       </c>
       <c r="D737" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E737" s="0" t="s">
         <v>458</v>
@@ -17651,7 +17652,7 @@
         <v>0.148995</v>
       </c>
       <c r="D738" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E738" s="0" t="s">
         <v>459</v>
@@ -17751,10 +17752,10 @@
         <v>0.148995</v>
       </c>
       <c r="D743" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E743" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E743" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F743" s="0" t="n">
         <v>0.003993</v>
@@ -17811,10 +17812,10 @@
         <v>0.148995</v>
       </c>
       <c r="D746" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E746" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E746" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F746" s="0" t="n">
         <v>0.003993</v>
@@ -17871,10 +17872,10 @@
         <v>0.148995</v>
       </c>
       <c r="D749" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E749" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E749" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F749" s="0" t="n">
         <v>0.003993</v>
@@ -17951,10 +17952,10 @@
         <v>0.148995</v>
       </c>
       <c r="D753" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E753" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E753" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F753" s="0" t="n">
         <v>0.003129</v>
@@ -17971,10 +17972,10 @@
         <v>0.148995</v>
       </c>
       <c r="D754" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E754" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E754" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F754" s="0" t="n">
         <v>0.003129</v>
@@ -20231,7 +20232,7 @@
         <v>0.149001</v>
       </c>
       <c r="D867" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E867" s="0" t="s">
         <v>456</v>
@@ -20331,7 +20332,7 @@
         <v>0.149001</v>
       </c>
       <c r="D872" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E872" s="0" t="s">
         <v>457</v>
@@ -20351,7 +20352,7 @@
         <v>0.149001</v>
       </c>
       <c r="D873" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E873" s="0" t="s">
         <v>458</v>
@@ -20371,7 +20372,7 @@
         <v>0.149001</v>
       </c>
       <c r="D874" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E874" s="0" t="s">
         <v>459</v>
@@ -20471,10 +20472,10 @@
         <v>0.149001</v>
       </c>
       <c r="D879" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E879" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E879" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F879" s="0" t="n">
         <v>0.003993</v>
@@ -20531,10 +20532,10 @@
         <v>0.149001</v>
       </c>
       <c r="D882" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E882" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E882" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F882" s="0" t="n">
         <v>0.003993</v>
@@ -20611,10 +20612,10 @@
         <v>0.149001</v>
       </c>
       <c r="D886" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E886" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E886" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F886" s="0" t="n">
         <v>0.003829</v>
@@ -20631,10 +20632,10 @@
         <v>0.149001</v>
       </c>
       <c r="D887" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E887" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E887" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F887" s="0" t="n">
         <v>0.003829</v>
@@ -20691,10 +20692,10 @@
         <v>0.149001</v>
       </c>
       <c r="D890" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E890" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E890" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F890" s="0" t="n">
         <v>0.003829</v>
@@ -22711,7 +22712,7 @@
         <v>0.148994</v>
       </c>
       <c r="D991" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E991" s="0" t="s">
         <v>456</v>
@@ -22811,7 +22812,7 @@
         <v>0.148994</v>
       </c>
       <c r="D996" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E996" s="0" t="s">
         <v>457</v>
@@ -22831,7 +22832,7 @@
         <v>0.148994</v>
       </c>
       <c r="D997" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E997" s="0" t="s">
         <v>458</v>
@@ -22851,7 +22852,7 @@
         <v>0.148994</v>
       </c>
       <c r="D998" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E998" s="0" t="s">
         <v>459</v>
@@ -22951,10 +22952,10 @@
         <v>0.148994</v>
       </c>
       <c r="D1003" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E1003" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E1003" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F1003" s="0" t="n">
         <v>0.003993</v>
@@ -23011,10 +23012,10 @@
         <v>0.148994</v>
       </c>
       <c r="D1006" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1006" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E1006" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F1006" s="0" t="n">
         <v>0.003993</v>
@@ -23071,10 +23072,10 @@
         <v>0.148994</v>
       </c>
       <c r="D1009" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1009" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E1009" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F1009" s="0" t="n">
         <v>0.003993</v>
@@ -23131,10 +23132,10 @@
         <v>0.148994</v>
       </c>
       <c r="D1012" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1012" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E1012" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F1012" s="0" t="n">
         <v>0.003337</v>
@@ -23151,10 +23152,10 @@
         <v>0.148994</v>
       </c>
       <c r="D1013" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E1013" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E1013" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F1013" s="0" t="n">
         <v>0.003337</v>
@@ -25151,7 +25152,7 @@
         <v>0.110118</v>
       </c>
       <c r="D1113" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E1113" s="0" t="s">
         <v>456</v>
@@ -25331,7 +25332,7 @@
         <v>0.110118</v>
       </c>
       <c r="D1122" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E1122" s="0" t="s">
         <v>459</v>
@@ -25451,10 +25452,10 @@
         <v>0.110118</v>
       </c>
       <c r="D1128" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1128" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E1128" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F1128" s="0" t="n">
         <v>0.002301</v>
@@ -25471,10 +25472,10 @@
         <v>0.110118</v>
       </c>
       <c r="D1129" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E1129" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E1129" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F1129" s="0" t="n">
         <v>0.002301</v>
@@ -25491,7 +25492,7 @@
         <v>0.110118</v>
       </c>
       <c r="D1130" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E1130" s="0" t="s">
         <v>457</v>
@@ -25551,10 +25552,10 @@
         <v>0.110118</v>
       </c>
       <c r="D1133" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1133" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="E1133" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="F1133" s="0" t="n">
         <v>0.001971</v>
@@ -25611,7 +25612,7 @@
         <v>0.110118</v>
       </c>
       <c r="D1136" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E1136" s="0" t="s">
         <v>458</v>
@@ -25851,10 +25852,10 @@
         <v>0.110118</v>
       </c>
       <c r="D1148" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1148" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E1148" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F1148" s="0" t="n">
         <v>0.001971</v>
@@ -25871,10 +25872,10 @@
         <v>0.110118</v>
       </c>
       <c r="D1149" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E1149" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E1149" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F1149" s="0" t="n">
         <v>0.001971</v>
@@ -25931,10 +25932,10 @@
         <v>0.110118</v>
       </c>
       <c r="D1152" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1152" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E1152" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F1152" s="0" t="n">
         <v>0.001971</v>
@@ -26131,10 +26132,10 @@
         <v>0.020206</v>
       </c>
       <c r="D1162" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1162" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="E1162" s="0" t="s">
-        <v>365</v>
       </c>
       <c r="F1162" s="0" t="n">
         <v>0.001407</v>
@@ -26291,10 +26292,10 @@
         <v>0.018304</v>
       </c>
       <c r="D1170" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1170" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="E1170" s="0" t="s">
-        <v>367</v>
       </c>
       <c r="F1170" s="0" t="n">
         <v>0.001407</v>
@@ -29194,7 +29195,7 @@
         <v>844</v>
       </c>
       <c r="E1315" s="0" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F1315" s="0" t="n">
         <v>0</v>
@@ -30211,7 +30212,7 @@
         <v>0.110106</v>
       </c>
       <c r="D1366" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E1366" s="0" t="s">
         <v>456</v>
@@ -30431,7 +30432,7 @@
         <v>0.110106</v>
       </c>
       <c r="D1377" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E1377" s="0" t="s">
         <v>458</v>
@@ -30451,7 +30452,7 @@
         <v>0.110106</v>
       </c>
       <c r="D1378" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E1378" s="0" t="s">
         <v>459</v>
@@ -30491,10 +30492,10 @@
         <v>0.110106</v>
       </c>
       <c r="D1380" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1380" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E1380" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F1380" s="0" t="n">
         <v>0.002301</v>
@@ -30531,10 +30532,10 @@
         <v>0.110106</v>
       </c>
       <c r="D1382" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1382" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E1382" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F1382" s="0" t="n">
         <v>0.002301</v>
@@ -30571,7 +30572,7 @@
         <v>0.110106</v>
       </c>
       <c r="D1384" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E1384" s="0" t="s">
         <v>457</v>
@@ -30611,10 +30612,10 @@
         <v>0.110106</v>
       </c>
       <c r="D1386" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E1386" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E1386" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F1386" s="0" t="n">
         <v>0.00196</v>
@@ -30671,10 +30672,10 @@
         <v>0.110106</v>
       </c>
       <c r="D1389" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1389" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="E1389" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="F1389" s="0" t="n">
         <v>0.00196</v>
@@ -30871,10 +30872,10 @@
         <v>0.110106</v>
       </c>
       <c r="D1399" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E1399" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E1399" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F1399" s="0" t="n">
         <v>0.00196</v>
@@ -30951,10 +30952,10 @@
         <v>0.110106</v>
       </c>
       <c r="D1403" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1403" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E1403" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F1403" s="0" t="n">
         <v>0.00196</v>
@@ -31331,10 +31332,10 @@
         <v>0.016227</v>
       </c>
       <c r="D1422" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1422" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="E1422" s="0" t="s">
-        <v>367</v>
       </c>
       <c r="F1422" s="0" t="n">
         <v>0.001451</v>
@@ -34234,7 +34235,7 @@
         <v>844</v>
       </c>
       <c r="E1567" s="0" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F1567" s="0" t="n">
         <v>0</v>
@@ -35251,7 +35252,7 @@
         <v>0.110098</v>
       </c>
       <c r="D1618" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E1618" s="0" t="s">
         <v>456</v>
@@ -35371,7 +35372,7 @@
         <v>0.110098</v>
       </c>
       <c r="D1624" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E1624" s="0" t="s">
         <v>459</v>
@@ -35551,10 +35552,10 @@
         <v>0.110098</v>
       </c>
       <c r="D1633" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1633" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E1633" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F1633" s="0" t="n">
         <v>0.002896</v>
@@ -35591,10 +35592,10 @@
         <v>0.110098</v>
       </c>
       <c r="D1635" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1635" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="E1635" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="F1635" s="0" t="n">
         <v>0.002103</v>
@@ -35611,10 +35612,10 @@
         <v>0.110098</v>
       </c>
       <c r="D1636" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1636" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E1636" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F1636" s="0" t="n">
         <v>0.002103</v>
@@ -35671,10 +35672,10 @@
         <v>0.110098</v>
       </c>
       <c r="D1639" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E1639" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E1639" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F1639" s="0" t="n">
         <v>0.002103</v>
@@ -35771,7 +35772,7 @@
         <v>0.110098</v>
       </c>
       <c r="D1644" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E1644" s="0" t="s">
         <v>457</v>
@@ -35831,7 +35832,7 @@
         <v>0.110098</v>
       </c>
       <c r="D1647" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E1647" s="0" t="s">
         <v>458</v>
@@ -35931,10 +35932,10 @@
         <v>0.110098</v>
       </c>
       <c r="D1652" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1652" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E1652" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F1652" s="0" t="n">
         <v>0.002103</v>
@@ -35951,10 +35952,10 @@
         <v>0.110098</v>
       </c>
       <c r="D1653" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E1653" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E1653" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F1653" s="0" t="n">
         <v>0.002103</v>
@@ -36111,10 +36112,10 @@
         <v>0.024123</v>
       </c>
       <c r="D1661" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1661" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="E1661" s="0" t="s">
-        <v>365</v>
       </c>
       <c r="F1661" s="0" t="n">
         <v>0.002045</v>
@@ -36271,10 +36272,10 @@
         <v>0.020891</v>
       </c>
       <c r="D1669" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1669" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="E1669" s="0" t="s">
-        <v>367</v>
       </c>
       <c r="F1669" s="0" t="n">
         <v>0.002045</v>
@@ -38274,7 +38275,7 @@
         <v>844</v>
       </c>
       <c r="E1769" s="0" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F1769" s="0" t="n">
         <v>0</v>
@@ -39271,7 +39272,7 @@
         <v>0.110096</v>
       </c>
       <c r="D1819" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E1819" s="0" t="s">
         <v>456</v>
@@ -39391,7 +39392,7 @@
         <v>0.110096</v>
       </c>
       <c r="D1825" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E1825" s="0" t="s">
         <v>459</v>
@@ -39471,7 +39472,7 @@
         <v>0.110096</v>
       </c>
       <c r="D1829" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E1829" s="0" t="s">
         <v>457</v>
@@ -39551,10 +39552,10 @@
         <v>0.110096</v>
       </c>
       <c r="D1833" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="E1833" s="0" t="s">
         <v>362</v>
-      </c>
-      <c r="E1833" s="0" t="s">
-        <v>363</v>
       </c>
       <c r="F1833" s="0" t="n">
         <v>0.002896</v>
@@ -39591,7 +39592,7 @@
         <v>0.110096</v>
       </c>
       <c r="D1835" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E1835" s="0" t="s">
         <v>458</v>
@@ -39651,10 +39652,10 @@
         <v>0.110096</v>
       </c>
       <c r="D1838" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="E1838" s="0" t="s">
         <v>360</v>
-      </c>
-      <c r="E1838" s="0" t="s">
-        <v>361</v>
       </c>
       <c r="F1838" s="0" t="n">
         <v>0.002059</v>
@@ -39691,10 +39692,10 @@
         <v>0.110096</v>
       </c>
       <c r="D1840" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1840" s="0" t="s">
         <v>351</v>
-      </c>
-      <c r="E1840" s="0" t="s">
-        <v>352</v>
       </c>
       <c r="F1840" s="0" t="n">
         <v>0.002059</v>
@@ -39871,10 +39872,10 @@
         <v>0.110096</v>
       </c>
       <c r="D1849" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1849" s="0" t="s">
         <v>349</v>
-      </c>
-      <c r="E1849" s="0" t="s">
-        <v>350</v>
       </c>
       <c r="F1849" s="0" t="n">
         <v>0.002059</v>
@@ -39931,10 +39932,10 @@
         <v>0.110096</v>
       </c>
       <c r="D1852" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="E1852" s="0" t="s">
         <v>356</v>
-      </c>
-      <c r="E1852" s="0" t="s">
-        <v>357</v>
       </c>
       <c r="F1852" s="0" t="n">
         <v>0.002059</v>
@@ -39971,10 +39972,10 @@
         <v>0.110096</v>
       </c>
       <c r="D1854" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E1854" s="0" t="s">
         <v>353</v>
-      </c>
-      <c r="E1854" s="0" t="s">
-        <v>354</v>
       </c>
       <c r="F1854" s="0" t="n">
         <v>0.002059</v>
@@ -40271,10 +40272,10 @@
         <v>0.01845</v>
       </c>
       <c r="D1869" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="E1869" s="0" t="s">
         <v>366</v>
-      </c>
-      <c r="E1869" s="0" t="s">
-        <v>367</v>
       </c>
       <c r="F1869" s="0" t="n">
         <v>0.002111</v>

</xml_diff>

<commit_message>
SD-66822 - CCRU - Template changes
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/KPIs for DB - PoS 2019.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/KPIs for DB - PoS 2019.xlsx
@@ -13,13 +13,14 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$2008</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$H$2008</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$2008</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -57,271 +58,271 @@
     <t xml:space="preserve">Tea Availability</t>
   </si>
   <si>
+    <t xml:space="preserve">Fuze Peach-Rose - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Petroleum - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Ultra - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Petroleum - REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Монстер Ультра - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - MT Hypermarket - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Mojito - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Level 3 Display Text RUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.25л слим</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Bitter Lemon - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Биттер Лемон - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Tonic - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Тоник - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Pear - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Груша - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.25л слим</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero Cherry - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро Вишня - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero Cherry - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро Вишня - 0.25л слим</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 0.25л слим</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.25л слим</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Bitter Lemon - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Биттер Лемон - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Pear - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Груша - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Tonic - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Тоник - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Carb - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Газ - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Viva - Lemon - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Вива - Лимон - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Carb - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Газ - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Green - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Монстер Грин - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Rossi - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Монстер Росси - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Apple Kiwi - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Берн Яблоко-Киви - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Berry-Hibiscus - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Лесн.ягоды - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Mango-Camomile - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Манго-Ромашка - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Lemon-Lemongrass - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Лимон - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Green Strawberry-Raspberry - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Зеленый Клубника-Малина - 0.5л</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fuze Berry-Hibiscus - 1L</t>
   </si>
   <si>
-    <t xml:space="preserve">PoS 2019 - IC Petroleum - CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monster Ultra - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoS 2019 - IC Petroleum - REG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Монстер Ультра - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoS 2019 - MT Hypermarket - CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Mojito - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI Level 3 Display Text RUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola - 0.25L Slim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола - 0.25л слим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Апельсин - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Апельсин - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola - 1.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола - 1.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola - 2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола - 2л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Bitter Lemon - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Биттер Лемон - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Tonic - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Тоник - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Pear - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Груша - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero - 0.25L Slim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро - 0.25л слим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero Cherry - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро Вишня - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero Cherry - 0.25L Slim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро Вишня - 0.25л слим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Orange - 0.25L Slim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Апельсин - 0.25л слим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite - 0.25L Slim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 0.25л слим</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Bitter Lemon - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Биттер Лемон - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fanta Pear - 0.9L/1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фанта Груша - 0.9л/1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Tonic - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Тоник - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Still - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Негаз - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Still - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Негаз - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Carb - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Газ - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Viva - Lemon - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Вива - Лимон - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Carb - 1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Газ - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Still - 2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Негаз - 2л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn Original - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn Original - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monster Green - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Монстер Грин - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monster Rossi - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Монстер Росси - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn Apple Kiwi - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Берн Яблоко-Киви - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn Original - 0.33L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn Original - 0.33л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuze Berry-Hibiscus - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фьюз Лесн.ягоды - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuze Mango-Camomile - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фьюз Манго-Ромашка - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuze Lemon-Lemongrass - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фьюз Лимон - 0.5л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuze Green Strawberry-Raspberry - 0.5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фьюз Зеленый Клубника-Малина - 0.5л</t>
-  </si>
-  <si>
     <t xml:space="preserve">Фьюз Лесн.ягоды - 1л</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuze Peach-Rose - 0.33L</t>
   </si>
   <si>
     <t xml:space="preserve">Фьюз Персик - 0.33л</t>
@@ -2855,18 +2856,16 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.6326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2988,18 +2987,18 @@
   <dimension ref="1:2008"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3922,7 +3921,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>6</v>
       </c>
@@ -3933,22 +3932,19 @@
         <v>0.046826</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>0.006501</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H40" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>6</v>
       </c>
@@ -3959,16 +3955,19 @@
         <v>0.046826</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>0.006501</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>97</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7547,16 +7546,16 @@
         <v>0.03496</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E197" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F197" s="0" t="n">
         <v>0.006992</v>
       </c>
       <c r="G197" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7570,10 +7569,10 @@
         <v>0.03496</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="E198" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="F198" s="0" t="n">
         <v>0.006992</v>
@@ -13530,10 +13529,10 @@
         <v>0.040597</v>
       </c>
       <c r="D457" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="E457" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="F457" s="0" t="n">
         <v>0.005597</v>
@@ -15120,10 +15119,10 @@
         <v>0.040626</v>
       </c>
       <c r="D526" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="E526" s="0" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="F526" s="0" t="n">
         <v>0.005596</v>
@@ -17535,16 +17534,16 @@
         <v>0.019634</v>
       </c>
       <c r="D631" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E631" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F631" s="0" t="n">
         <v>0.003992</v>
       </c>
       <c r="G631" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="632" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20787,7 +20786,7 @@
         <v>0.001662</v>
       </c>
       <c r="G772" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="773" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23814,16 +23813,16 @@
         <v>0.017187</v>
       </c>
       <c r="D904" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E904" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F904" s="0" t="n">
         <v>0.003992</v>
       </c>
       <c r="G904" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="905" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26620,16 +26619,16 @@
         <v>0.015796</v>
       </c>
       <c r="D1026" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E1026" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F1026" s="0" t="n">
         <v>0.00191</v>
       </c>
       <c r="G1026" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="1027" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30211,16 +30210,16 @@
         <v>0.024713</v>
       </c>
       <c r="D1182" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E1182" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F1182" s="0" t="n">
         <v>0.001407</v>
       </c>
       <c r="G1182" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="1183" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36007,16 +36006,16 @@
         <v>0.025153</v>
       </c>
       <c r="D1434" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E1434" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F1434" s="0" t="n">
         <v>0.001451</v>
       </c>
       <c r="G1434" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="1435" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41711,16 +41710,16 @@
         <v>0.023882</v>
       </c>
       <c r="D1682" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E1682" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F1682" s="0" t="n">
         <v>0.002045</v>
       </c>
       <c r="G1682" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="1683" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46288,16 +46287,16 @@
         <v>0.024278</v>
       </c>
       <c r="D1881" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E1881" s="0" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="F1881" s="0" t="n">
         <v>0.002111</v>
       </c>
       <c r="G1881" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="1882" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>